<commit_message>
Mosip 29878  Added registration center Data for spanish language (#277)
* MOSIP-29878 Added spanish language data for reg center and zone.

Signed-off-by: kameshsr <kameshsr1338@gmail.com>

* MOSIP-29878 Added spanish language data for reg center.

Signed-off-by: kameshsr <kameshsr1338@gmail.com>

* updated Registration center for spanish language.

Signed-off-by: kameshsr <kameshsr1338@gmail.com>

* added days of week for spanish language

Signed-off-by: kameshsr <kameshsr1338@gmail.com>

* added registration center working days for spanish language

Signed-off-by: kameshsr <kameshsr1338@gmail.com>

* added registration center template for spanish language

Signed-off-by: kameshsr <kameshsr1338@gmail.com>

---------

Signed-off-by: kameshsr <kameshsr1338@gmail.com>
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/reg_working_nonworking.xlsx
+++ b/mosip_master/xlsx/reg_working_nonworking.xlsx
@@ -1,16 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kames\IdeaProjects\mosip-data\mosip_master\xlsx\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5552E58F-5F33-466F-932A-0E6ED4B72993}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -20,41 +25,61 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="16">
   <si>
-    <t xml:space="preserve">lang_code</t>
+    <t>lang_code</t>
   </si>
   <si>
-    <t xml:space="preserve">regcntr_id</t>
+    <t>regcntr_id</t>
   </si>
   <si>
-    <t xml:space="preserve">day_code</t>
+    <t>day_code</t>
   </si>
   <si>
-    <t xml:space="preserve">is_working</t>
+    <t>is_working</t>
   </si>
   <si>
-    <t xml:space="preserve">is_active</t>
+    <t>is_active</t>
   </si>
   <si>
-    <t xml:space="preserve">eng</t>
+    <t>eng</t>
   </si>
   <si>
-    <t xml:space="preserve">FALSE</t>
+    <t>FALSE</t>
   </si>
   <si>
-    <t xml:space="preserve">TRUE</t>
+    <t>TRUE</t>
+  </si>
+  <si>
+    <t>10151</t>
+  </si>
+  <si>
+    <t>10152</t>
+  </si>
+  <si>
+    <t>10153</t>
+  </si>
+  <si>
+    <t>10154</t>
+  </si>
+  <si>
+    <t>10155</t>
+  </si>
+  <si>
+    <t>10156</t>
+  </si>
+  <si>
+    <t>10157</t>
+  </si>
+  <si>
+    <t>spa</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="@"/>
-  </numFmts>
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -63,25 +88,9 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <name val="Cambria"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
@@ -89,6 +98,12 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -100,100 +115,368 @@
     </fill>
   </fills>
   <borders count="2">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  </cellStyleXfs>
+  <cellXfs count="5">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-  </cellStyleXfs>
-  <cellXfs count="6">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:E106"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E113"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D99" activeCellId="0" sqref="D99"/>
+    <sheetView tabSelected="1" topLeftCell="A97" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G112" sqref="G112"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="2" style="1" width="8.43"/>
+    <col min="2" max="5" width="8.453125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -210,14 +493,14 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="1" t="n">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1">
         <v>10001</v>
       </c>
-      <c r="C2" s="1" t="n">
+      <c r="C2" s="1">
         <v>101</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -227,14 +510,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="1" t="n">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1">
         <v>10001</v>
       </c>
-      <c r="C3" s="1" t="n">
+      <c r="C3" s="1">
         <v>102</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -244,14 +527,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="1" t="n">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1">
         <v>10001</v>
       </c>
-      <c r="C4" s="1" t="n">
+      <c r="C4" s="1">
         <v>103</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -261,14 +544,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="1" t="n">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1">
         <v>10001</v>
       </c>
-      <c r="C5" s="1" t="n">
+      <c r="C5" s="1">
         <v>104</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -278,14 +561,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="n">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1">
         <v>10001</v>
       </c>
-      <c r="C6" s="1" t="n">
+      <c r="C6" s="1">
         <v>105</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -295,14 +578,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="1" t="n">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1">
         <v>10001</v>
       </c>
-      <c r="C7" s="1" t="n">
+      <c r="C7" s="1">
         <v>106</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -312,14 +595,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="1" t="n">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="1">
         <v>10001</v>
       </c>
-      <c r="C8" s="1" t="n">
+      <c r="C8" s="1">
         <v>107</v>
       </c>
       <c r="D8" s="1" t="s">
@@ -329,14 +612,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" s="1" t="n">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="1">
         <v>10002</v>
       </c>
-      <c r="C9" s="1" t="n">
+      <c r="C9" s="1">
         <v>101</v>
       </c>
       <c r="D9" s="1" t="s">
@@ -346,14 +629,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" s="1" t="n">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="1">
         <v>10002</v>
       </c>
-      <c r="C10" s="1" t="n">
+      <c r="C10" s="1">
         <v>102</v>
       </c>
       <c r="D10" s="1" t="s">
@@ -363,14 +646,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" s="1" t="n">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="1">
         <v>10002</v>
       </c>
-      <c r="C11" s="1" t="n">
+      <c r="C11" s="1">
         <v>103</v>
       </c>
       <c r="D11" s="1" t="s">
@@ -380,14 +663,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12" s="1" t="n">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="1">
         <v>10002</v>
       </c>
-      <c r="C12" s="1" t="n">
+      <c r="C12" s="1">
         <v>104</v>
       </c>
       <c r="D12" s="1" t="s">
@@ -397,14 +680,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B13" s="1" t="n">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="1">
         <v>10002</v>
       </c>
-      <c r="C13" s="1" t="n">
+      <c r="C13" s="1">
         <v>105</v>
       </c>
       <c r="D13" s="1" t="s">
@@ -414,14 +697,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B14" s="1" t="n">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="1">
         <v>10002</v>
       </c>
-      <c r="C14" s="1" t="n">
+      <c r="C14" s="1">
         <v>106</v>
       </c>
       <c r="D14" s="1" t="s">
@@ -431,14 +714,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B15" s="1" t="n">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="1">
         <v>10002</v>
       </c>
-      <c r="C15" s="1" t="n">
+      <c r="C15" s="1">
         <v>107</v>
       </c>
       <c r="D15" s="1" t="s">
@@ -448,14 +731,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B16" s="1" t="n">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="1">
         <v>10003</v>
       </c>
-      <c r="C16" s="1" t="n">
+      <c r="C16" s="1">
         <v>101</v>
       </c>
       <c r="D16" s="1" t="s">
@@ -465,14 +748,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B17" s="1" t="n">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="1">
         <v>10003</v>
       </c>
-      <c r="C17" s="1" t="n">
+      <c r="C17" s="1">
         <v>102</v>
       </c>
       <c r="D17" s="1" t="s">
@@ -482,14 +765,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B18" s="1" t="n">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="1">
         <v>10003</v>
       </c>
-      <c r="C18" s="1" t="n">
+      <c r="C18" s="1">
         <v>103</v>
       </c>
       <c r="D18" s="1" t="s">
@@ -499,14 +782,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B19" s="1" t="n">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" s="1">
         <v>10003</v>
       </c>
-      <c r="C19" s="1" t="n">
+      <c r="C19" s="1">
         <v>104</v>
       </c>
       <c r="D19" s="1" t="s">
@@ -516,14 +799,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B20" s="1" t="n">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" s="1">
         <v>10003</v>
       </c>
-      <c r="C20" s="1" t="n">
+      <c r="C20" s="1">
         <v>105</v>
       </c>
       <c r="D20" s="1" t="s">
@@ -533,14 +816,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B21" s="1" t="n">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" s="1">
         <v>10003</v>
       </c>
-      <c r="C21" s="1" t="n">
+      <c r="C21" s="1">
         <v>106</v>
       </c>
       <c r="D21" s="1" t="s">
@@ -550,14 +833,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B22" s="1" t="n">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" s="1">
         <v>10003</v>
       </c>
-      <c r="C22" s="1" t="n">
+      <c r="C22" s="1">
         <v>107</v>
       </c>
       <c r="D22" s="1" t="s">
@@ -567,14 +850,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B23" s="1" t="n">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23" s="1">
         <v>10004</v>
       </c>
-      <c r="C23" s="1" t="n">
+      <c r="C23" s="1">
         <v>101</v>
       </c>
       <c r="D23" s="1" t="s">
@@ -584,14 +867,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B24" s="1" t="n">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" s="1">
         <v>10004</v>
       </c>
-      <c r="C24" s="1" t="n">
+      <c r="C24" s="1">
         <v>102</v>
       </c>
       <c r="D24" s="1" t="s">
@@ -601,14 +884,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B25" s="1" t="n">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25" s="1">
         <v>10004</v>
       </c>
-      <c r="C25" s="1" t="n">
+      <c r="C25" s="1">
         <v>103</v>
       </c>
       <c r="D25" s="1" t="s">
@@ -618,14 +901,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B26" s="1" t="n">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" s="1">
         <v>10004</v>
       </c>
-      <c r="C26" s="1" t="n">
+      <c r="C26" s="1">
         <v>104</v>
       </c>
       <c r="D26" s="1" t="s">
@@ -635,14 +918,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B27" s="1" t="n">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27" s="1">
         <v>10004</v>
       </c>
-      <c r="C27" s="1" t="n">
+      <c r="C27" s="1">
         <v>105</v>
       </c>
       <c r="D27" s="1" t="s">
@@ -652,14 +935,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B28" s="1" t="n">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>5</v>
+      </c>
+      <c r="B28" s="1">
         <v>10004</v>
       </c>
-      <c r="C28" s="1" t="n">
+      <c r="C28" s="1">
         <v>106</v>
       </c>
       <c r="D28" s="1" t="s">
@@ -669,14 +952,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B29" s="1" t="n">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29" s="1">
         <v>10004</v>
       </c>
-      <c r="C29" s="1" t="n">
+      <c r="C29" s="1">
         <v>107</v>
       </c>
       <c r="D29" s="1" t="s">
@@ -686,14 +969,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B30" s="1" t="n">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>5</v>
+      </c>
+      <c r="B30" s="1">
         <v>10005</v>
       </c>
-      <c r="C30" s="1" t="n">
+      <c r="C30" s="1">
         <v>101</v>
       </c>
       <c r="D30" s="1" t="s">
@@ -703,14 +986,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B31" s="1" t="n">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31" s="1">
         <v>10005</v>
       </c>
-      <c r="C31" s="1" t="n">
+      <c r="C31" s="1">
         <v>102</v>
       </c>
       <c r="D31" s="1" t="s">
@@ -720,14 +1003,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B32" s="1" t="n">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>5</v>
+      </c>
+      <c r="B32" s="1">
         <v>10005</v>
       </c>
-      <c r="C32" s="1" t="n">
+      <c r="C32" s="1">
         <v>103</v>
       </c>
       <c r="D32" s="1" t="s">
@@ -737,14 +1020,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B33" s="1" t="n">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>5</v>
+      </c>
+      <c r="B33" s="1">
         <v>10005</v>
       </c>
-      <c r="C33" s="1" t="n">
+      <c r="C33" s="1">
         <v>104</v>
       </c>
       <c r="D33" s="1" t="s">
@@ -754,14 +1037,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B34" s="1" t="n">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>5</v>
+      </c>
+      <c r="B34" s="1">
         <v>10005</v>
       </c>
-      <c r="C34" s="1" t="n">
+      <c r="C34" s="1">
         <v>105</v>
       </c>
       <c r="D34" s="1" t="s">
@@ -771,14 +1054,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B35" s="1" t="n">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>5</v>
+      </c>
+      <c r="B35" s="1">
         <v>10005</v>
       </c>
-      <c r="C35" s="1" t="n">
+      <c r="C35" s="1">
         <v>106</v>
       </c>
       <c r="D35" s="1" t="s">
@@ -788,14 +1071,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B36" s="1" t="n">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>5</v>
+      </c>
+      <c r="B36" s="1">
         <v>10005</v>
       </c>
-      <c r="C36" s="1" t="n">
+      <c r="C36" s="1">
         <v>107</v>
       </c>
       <c r="D36" s="1" t="s">
@@ -805,14 +1088,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B37" s="1" t="n">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>5</v>
+      </c>
+      <c r="B37" s="1">
         <v>10006</v>
       </c>
-      <c r="C37" s="1" t="n">
+      <c r="C37" s="1">
         <v>101</v>
       </c>
       <c r="D37" s="1" t="s">
@@ -822,14 +1105,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B38" s="1" t="n">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>5</v>
+      </c>
+      <c r="B38" s="1">
         <v>10006</v>
       </c>
-      <c r="C38" s="1" t="n">
+      <c r="C38" s="1">
         <v>102</v>
       </c>
       <c r="D38" s="1" t="s">
@@ -839,14 +1122,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B39" s="1" t="n">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>5</v>
+      </c>
+      <c r="B39" s="1">
         <v>10006</v>
       </c>
-      <c r="C39" s="1" t="n">
+      <c r="C39" s="1">
         <v>103</v>
       </c>
       <c r="D39" s="1" t="s">
@@ -856,14 +1139,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B40" s="1" t="n">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>5</v>
+      </c>
+      <c r="B40" s="1">
         <v>10006</v>
       </c>
-      <c r="C40" s="1" t="n">
+      <c r="C40" s="1">
         <v>104</v>
       </c>
       <c r="D40" s="1" t="s">
@@ -873,14 +1156,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B41" s="1" t="n">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>5</v>
+      </c>
+      <c r="B41" s="1">
         <v>10006</v>
       </c>
-      <c r="C41" s="1" t="n">
+      <c r="C41" s="1">
         <v>105</v>
       </c>
       <c r="D41" s="1" t="s">
@@ -890,14 +1173,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B42" s="1" t="n">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>5</v>
+      </c>
+      <c r="B42" s="1">
         <v>10006</v>
       </c>
-      <c r="C42" s="1" t="n">
+      <c r="C42" s="1">
         <v>106</v>
       </c>
       <c r="D42" s="1" t="s">
@@ -907,14 +1190,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B43" s="1" t="n">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>5</v>
+      </c>
+      <c r="B43" s="1">
         <v>10006</v>
       </c>
-      <c r="C43" s="1" t="n">
+      <c r="C43" s="1">
         <v>107</v>
       </c>
       <c r="D43" s="1" t="s">
@@ -924,14 +1207,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B44" s="1" t="n">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>5</v>
+      </c>
+      <c r="B44" s="1">
         <v>10007</v>
       </c>
-      <c r="C44" s="1" t="n">
+      <c r="C44" s="1">
         <v>101</v>
       </c>
       <c r="D44" s="1" t="s">
@@ -941,14 +1224,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B45" s="1" t="n">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>5</v>
+      </c>
+      <c r="B45" s="1">
         <v>10007</v>
       </c>
-      <c r="C45" s="1" t="n">
+      <c r="C45" s="1">
         <v>102</v>
       </c>
       <c r="D45" s="1" t="s">
@@ -958,14 +1241,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B46" s="1" t="n">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>5</v>
+      </c>
+      <c r="B46" s="1">
         <v>10007</v>
       </c>
-      <c r="C46" s="1" t="n">
+      <c r="C46" s="1">
         <v>103</v>
       </c>
       <c r="D46" s="1" t="s">
@@ -975,14 +1258,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B47" s="1" t="n">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>5</v>
+      </c>
+      <c r="B47" s="1">
         <v>10007</v>
       </c>
-      <c r="C47" s="1" t="n">
+      <c r="C47" s="1">
         <v>104</v>
       </c>
       <c r="D47" s="1" t="s">
@@ -992,14 +1275,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B48" s="1" t="n">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>5</v>
+      </c>
+      <c r="B48" s="1">
         <v>10007</v>
       </c>
-      <c r="C48" s="1" t="n">
+      <c r="C48" s="1">
         <v>105</v>
       </c>
       <c r="D48" s="1" t="s">
@@ -1009,14 +1292,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B49" s="1" t="n">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>5</v>
+      </c>
+      <c r="B49" s="1">
         <v>10007</v>
       </c>
-      <c r="C49" s="1" t="n">
+      <c r="C49" s="1">
         <v>106</v>
       </c>
       <c r="D49" s="1" t="s">
@@ -1026,14 +1309,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B50" s="1" t="n">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>5</v>
+      </c>
+      <c r="B50" s="1">
         <v>10007</v>
       </c>
-      <c r="C50" s="1" t="n">
+      <c r="C50" s="1">
         <v>107</v>
       </c>
       <c r="D50" s="1" t="s">
@@ -1043,14 +1326,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B51" s="1" t="n">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>5</v>
+      </c>
+      <c r="B51" s="1">
         <v>10008</v>
       </c>
-      <c r="C51" s="1" t="n">
+      <c r="C51" s="1">
         <v>101</v>
       </c>
       <c r="D51" s="1" t="s">
@@ -1060,99 +1343,99 @@
         <v>7</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B52" s="1" t="n">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>5</v>
+      </c>
+      <c r="B52" s="1">
         <v>10008</v>
       </c>
-      <c r="C52" s="1" t="n">
+      <c r="C52" s="1">
         <v>102</v>
       </c>
-      <c r="D52" s="5" t="s">
+      <c r="D52" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B53" s="1" t="n">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>5</v>
+      </c>
+      <c r="B53" s="1">
         <v>10008</v>
       </c>
-      <c r="C53" s="1" t="n">
+      <c r="C53" s="1">
         <v>103</v>
       </c>
-      <c r="D53" s="5" t="s">
+      <c r="D53" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B54" s="1" t="n">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>5</v>
+      </c>
+      <c r="B54" s="1">
         <v>10008</v>
       </c>
-      <c r="C54" s="1" t="n">
+      <c r="C54" s="1">
         <v>104</v>
       </c>
-      <c r="D54" s="5" t="s">
+      <c r="D54" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B55" s="1" t="n">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>5</v>
+      </c>
+      <c r="B55" s="1">
         <v>10008</v>
       </c>
-      <c r="C55" s="1" t="n">
+      <c r="C55" s="1">
         <v>105</v>
       </c>
-      <c r="D55" s="5" t="s">
+      <c r="D55" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B56" s="1" t="n">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>5</v>
+      </c>
+      <c r="B56" s="1">
         <v>10008</v>
       </c>
-      <c r="C56" s="1" t="n">
+      <c r="C56" s="1">
         <v>106</v>
       </c>
-      <c r="D56" s="5" t="s">
+      <c r="D56" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B57" s="1" t="n">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>5</v>
+      </c>
+      <c r="B57" s="1">
         <v>10008</v>
       </c>
-      <c r="C57" s="1" t="n">
+      <c r="C57" s="1">
         <v>107</v>
       </c>
       <c r="D57" s="1" t="s">
@@ -1162,14 +1445,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B58" s="1" t="n">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>5</v>
+      </c>
+      <c r="B58" s="1">
         <v>10009</v>
       </c>
-      <c r="C58" s="1" t="n">
+      <c r="C58" s="1">
         <v>101</v>
       </c>
       <c r="D58" s="1" t="s">
@@ -1179,14 +1462,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B59" s="1" t="n">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>5</v>
+      </c>
+      <c r="B59" s="1">
         <v>10009</v>
       </c>
-      <c r="C59" s="1" t="n">
+      <c r="C59" s="1">
         <v>102</v>
       </c>
       <c r="D59" s="1" t="s">
@@ -1196,14 +1479,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B60" s="1" t="n">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>5</v>
+      </c>
+      <c r="B60" s="1">
         <v>10009</v>
       </c>
-      <c r="C60" s="1" t="n">
+      <c r="C60" s="1">
         <v>103</v>
       </c>
       <c r="D60" s="1" t="s">
@@ -1213,14 +1496,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B61" s="1" t="n">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>5</v>
+      </c>
+      <c r="B61" s="1">
         <v>10009</v>
       </c>
-      <c r="C61" s="1" t="n">
+      <c r="C61" s="1">
         <v>104</v>
       </c>
       <c r="D61" s="1" t="s">
@@ -1230,14 +1513,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B62" s="1" t="n">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>5</v>
+      </c>
+      <c r="B62" s="1">
         <v>10009</v>
       </c>
-      <c r="C62" s="1" t="n">
+      <c r="C62" s="1">
         <v>105</v>
       </c>
       <c r="D62" s="1" t="s">
@@ -1247,14 +1530,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B63" s="1" t="n">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>5</v>
+      </c>
+      <c r="B63" s="1">
         <v>10009</v>
       </c>
-      <c r="C63" s="1" t="n">
+      <c r="C63" s="1">
         <v>106</v>
       </c>
       <c r="D63" s="1" t="s">
@@ -1264,14 +1547,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B64" s="1" t="n">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>5</v>
+      </c>
+      <c r="B64" s="1">
         <v>10009</v>
       </c>
-      <c r="C64" s="1" t="n">
+      <c r="C64" s="1">
         <v>107</v>
       </c>
       <c r="D64" s="1" t="s">
@@ -1281,14 +1564,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B65" s="1" t="n">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>5</v>
+      </c>
+      <c r="B65" s="1">
         <v>10010</v>
       </c>
-      <c r="C65" s="1" t="n">
+      <c r="C65" s="1">
         <v>101</v>
       </c>
       <c r="D65" s="1" t="s">
@@ -1298,14 +1581,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B66" s="1" t="n">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
+        <v>5</v>
+      </c>
+      <c r="B66" s="1">
         <v>10010</v>
       </c>
-      <c r="C66" s="1" t="n">
+      <c r="C66" s="1">
         <v>102</v>
       </c>
       <c r="D66" s="1" t="s">
@@ -1315,14 +1598,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B67" s="1" t="n">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
+        <v>5</v>
+      </c>
+      <c r="B67" s="1">
         <v>10010</v>
       </c>
-      <c r="C67" s="1" t="n">
+      <c r="C67" s="1">
         <v>103</v>
       </c>
       <c r="D67" s="1" t="s">
@@ -1332,14 +1615,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B68" s="1" t="n">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
+        <v>5</v>
+      </c>
+      <c r="B68" s="1">
         <v>10010</v>
       </c>
-      <c r="C68" s="1" t="n">
+      <c r="C68" s="1">
         <v>104</v>
       </c>
       <c r="D68" s="1" t="s">
@@ -1349,14 +1632,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B69" s="1" t="n">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
+        <v>5</v>
+      </c>
+      <c r="B69" s="1">
         <v>10010</v>
       </c>
-      <c r="C69" s="1" t="n">
+      <c r="C69" s="1">
         <v>105</v>
       </c>
       <c r="D69" s="1" t="s">
@@ -1366,14 +1649,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B70" s="1" t="n">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
+        <v>5</v>
+      </c>
+      <c r="B70" s="1">
         <v>10010</v>
       </c>
-      <c r="C70" s="1" t="n">
+      <c r="C70" s="1">
         <v>106</v>
       </c>
       <c r="D70" s="1" t="s">
@@ -1383,14 +1666,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B71" s="1" t="n">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
+        <v>5</v>
+      </c>
+      <c r="B71" s="1">
         <v>10010</v>
       </c>
-      <c r="C71" s="1" t="n">
+      <c r="C71" s="1">
         <v>107</v>
       </c>
       <c r="D71" s="1" t="s">
@@ -1400,14 +1683,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B72" s="1" t="n">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
+        <v>5</v>
+      </c>
+      <c r="B72" s="1">
         <v>10011</v>
       </c>
-      <c r="C72" s="1" t="n">
+      <c r="C72" s="1">
         <v>101</v>
       </c>
       <c r="D72" s="1" t="s">
@@ -1417,99 +1700,99 @@
         <v>7</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B73" s="1" t="n">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
+        <v>5</v>
+      </c>
+      <c r="B73" s="1">
         <v>10011</v>
       </c>
-      <c r="C73" s="1" t="n">
+      <c r="C73" s="1">
         <v>102</v>
       </c>
-      <c r="D73" s="5" t="s">
+      <c r="D73" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E73" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B74" s="1" t="n">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A74" t="s">
+        <v>5</v>
+      </c>
+      <c r="B74" s="1">
         <v>10011</v>
       </c>
-      <c r="C74" s="1" t="n">
+      <c r="C74" s="1">
         <v>103</v>
       </c>
-      <c r="D74" s="5" t="s">
+      <c r="D74" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E74" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B75" s="1" t="n">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A75" t="s">
+        <v>5</v>
+      </c>
+      <c r="B75" s="1">
         <v>10011</v>
       </c>
-      <c r="C75" s="1" t="n">
+      <c r="C75" s="1">
         <v>104</v>
       </c>
-      <c r="D75" s="5" t="s">
+      <c r="D75" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E75" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B76" s="1" t="n">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A76" t="s">
+        <v>5</v>
+      </c>
+      <c r="B76" s="1">
         <v>10011</v>
       </c>
-      <c r="C76" s="1" t="n">
+      <c r="C76" s="1">
         <v>105</v>
       </c>
-      <c r="D76" s="5" t="s">
+      <c r="D76" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E76" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B77" s="1" t="n">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A77" t="s">
+        <v>5</v>
+      </c>
+      <c r="B77" s="1">
         <v>10011</v>
       </c>
-      <c r="C77" s="1" t="n">
+      <c r="C77" s="1">
         <v>106</v>
       </c>
-      <c r="D77" s="5" t="s">
+      <c r="D77" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E77" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B78" s="1" t="n">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A78" t="s">
+        <v>5</v>
+      </c>
+      <c r="B78" s="1">
         <v>10011</v>
       </c>
-      <c r="C78" s="1" t="n">
+      <c r="C78" s="1">
         <v>107</v>
       </c>
       <c r="D78" s="1" t="s">
@@ -1519,14 +1802,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B79" s="1" t="n">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A79" t="s">
+        <v>5</v>
+      </c>
+      <c r="B79" s="1">
         <v>10012</v>
       </c>
-      <c r="C79" s="1" t="n">
+      <c r="C79" s="1">
         <v>101</v>
       </c>
       <c r="D79" s="1" t="s">
@@ -1536,14 +1819,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B80" s="1" t="n">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A80" t="s">
+        <v>5</v>
+      </c>
+      <c r="B80" s="1">
         <v>10012</v>
       </c>
-      <c r="C80" s="1" t="n">
+      <c r="C80" s="1">
         <v>102</v>
       </c>
       <c r="D80" s="1" t="s">
@@ -1553,14 +1836,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B81" s="1" t="n">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A81" t="s">
+        <v>5</v>
+      </c>
+      <c r="B81" s="1">
         <v>10012</v>
       </c>
-      <c r="C81" s="1" t="n">
+      <c r="C81" s="1">
         <v>103</v>
       </c>
       <c r="D81" s="1" t="s">
@@ -1570,14 +1853,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B82" s="1" t="n">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A82" t="s">
+        <v>5</v>
+      </c>
+      <c r="B82" s="1">
         <v>10012</v>
       </c>
-      <c r="C82" s="1" t="n">
+      <c r="C82" s="1">
         <v>104</v>
       </c>
       <c r="D82" s="1" t="s">
@@ -1587,14 +1870,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B83" s="1" t="n">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A83" t="s">
+        <v>5</v>
+      </c>
+      <c r="B83" s="1">
         <v>10012</v>
       </c>
-      <c r="C83" s="1" t="n">
+      <c r="C83" s="1">
         <v>105</v>
       </c>
       <c r="D83" s="1" t="s">
@@ -1604,14 +1887,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B84" s="1" t="n">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A84" t="s">
+        <v>5</v>
+      </c>
+      <c r="B84" s="1">
         <v>10012</v>
       </c>
-      <c r="C84" s="1" t="n">
+      <c r="C84" s="1">
         <v>106</v>
       </c>
       <c r="D84" s="1" t="s">
@@ -1621,14 +1904,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B85" s="1" t="n">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A85" t="s">
+        <v>5</v>
+      </c>
+      <c r="B85" s="1">
         <v>10012</v>
       </c>
-      <c r="C85" s="1" t="n">
+      <c r="C85" s="1">
         <v>107</v>
       </c>
       <c r="D85" s="1" t="s">
@@ -1638,14 +1921,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B86" s="1" t="n">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A86" t="s">
+        <v>5</v>
+      </c>
+      <c r="B86" s="1">
         <v>10013</v>
       </c>
-      <c r="C86" s="1" t="n">
+      <c r="C86" s="1">
         <v>101</v>
       </c>
       <c r="D86" s="1" t="s">
@@ -1655,14 +1938,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B87" s="1" t="n">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A87" t="s">
+        <v>5</v>
+      </c>
+      <c r="B87" s="1">
         <v>10013</v>
       </c>
-      <c r="C87" s="1" t="n">
+      <c r="C87" s="1">
         <v>102</v>
       </c>
       <c r="D87" s="1" t="s">
@@ -1672,14 +1955,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B88" s="1" t="n">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A88" t="s">
+        <v>5</v>
+      </c>
+      <c r="B88" s="1">
         <v>10013</v>
       </c>
-      <c r="C88" s="1" t="n">
+      <c r="C88" s="1">
         <v>103</v>
       </c>
       <c r="D88" s="1" t="s">
@@ -1689,14 +1972,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B89" s="1" t="n">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A89" t="s">
+        <v>5</v>
+      </c>
+      <c r="B89" s="1">
         <v>10013</v>
       </c>
-      <c r="C89" s="1" t="n">
+      <c r="C89" s="1">
         <v>104</v>
       </c>
       <c r="D89" s="1" t="s">
@@ -1706,14 +1989,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B90" s="1" t="n">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A90" t="s">
+        <v>5</v>
+      </c>
+      <c r="B90" s="1">
         <v>10013</v>
       </c>
-      <c r="C90" s="1" t="n">
+      <c r="C90" s="1">
         <v>105</v>
       </c>
       <c r="D90" s="1" t="s">
@@ -1723,14 +2006,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B91" s="1" t="n">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A91" t="s">
+        <v>5</v>
+      </c>
+      <c r="B91" s="1">
         <v>10013</v>
       </c>
-      <c r="C91" s="1" t="n">
+      <c r="C91" s="1">
         <v>106</v>
       </c>
       <c r="D91" s="1" t="s">
@@ -1740,14 +2023,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B92" s="1" t="n">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A92" t="s">
+        <v>5</v>
+      </c>
+      <c r="B92" s="1">
         <v>10013</v>
       </c>
-      <c r="C92" s="1" t="n">
+      <c r="C92" s="1">
         <v>107</v>
       </c>
       <c r="D92" s="1" t="s">
@@ -1757,14 +2040,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B93" s="1" t="n">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A93" t="s">
+        <v>5</v>
+      </c>
+      <c r="B93" s="1">
         <v>10014</v>
       </c>
-      <c r="C93" s="1" t="n">
+      <c r="C93" s="1">
         <v>101</v>
       </c>
       <c r="D93" s="1" t="s">
@@ -1774,14 +2057,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B94" s="1" t="n">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A94" t="s">
+        <v>5</v>
+      </c>
+      <c r="B94" s="1">
         <v>10014</v>
       </c>
-      <c r="C94" s="1" t="n">
+      <c r="C94" s="1">
         <v>102</v>
       </c>
       <c r="D94" s="1" t="s">
@@ -1791,14 +2074,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B95" s="1" t="n">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A95" t="s">
+        <v>5</v>
+      </c>
+      <c r="B95" s="1">
         <v>10014</v>
       </c>
-      <c r="C95" s="1" t="n">
+      <c r="C95" s="1">
         <v>103</v>
       </c>
       <c r="D95" s="1" t="s">
@@ -1808,14 +2091,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B96" s="1" t="n">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A96" t="s">
+        <v>5</v>
+      </c>
+      <c r="B96" s="1">
         <v>10014</v>
       </c>
-      <c r="C96" s="1" t="n">
+      <c r="C96" s="1">
         <v>104</v>
       </c>
       <c r="D96" s="1" t="s">
@@ -1825,14 +2108,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B97" s="1" t="n">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A97" t="s">
+        <v>5</v>
+      </c>
+      <c r="B97" s="1">
         <v>10014</v>
       </c>
-      <c r="C97" s="1" t="n">
+      <c r="C97" s="1">
         <v>105</v>
       </c>
       <c r="D97" s="1" t="s">
@@ -1842,14 +2125,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B98" s="1" t="n">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A98" t="s">
+        <v>5</v>
+      </c>
+      <c r="B98" s="1">
         <v>10014</v>
       </c>
-      <c r="C98" s="1" t="n">
+      <c r="C98" s="1">
         <v>106</v>
       </c>
       <c r="D98" s="1" t="s">
@@ -1859,14 +2142,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B99" s="1" t="n">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A99" t="s">
+        <v>5</v>
+      </c>
+      <c r="B99" s="1">
         <v>10014</v>
       </c>
-      <c r="C99" s="1" t="n">
+      <c r="C99" s="1">
         <v>107</v>
       </c>
       <c r="D99" s="1" t="s">
@@ -1876,14 +2159,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B100" s="1" t="n">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A100" t="s">
+        <v>5</v>
+      </c>
+      <c r="B100" s="1">
         <v>10015</v>
       </c>
-      <c r="C100" s="1" t="n">
+      <c r="C100" s="1">
         <v>101</v>
       </c>
       <c r="D100" s="1" t="s">
@@ -1893,14 +2176,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B101" s="1" t="n">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A101" t="s">
+        <v>5</v>
+      </c>
+      <c r="B101" s="1">
         <v>10015</v>
       </c>
-      <c r="C101" s="1" t="n">
+      <c r="C101" s="1">
         <v>102</v>
       </c>
       <c r="D101" s="1" t="s">
@@ -1910,14 +2193,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B102" s="1" t="n">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A102" t="s">
+        <v>5</v>
+      </c>
+      <c r="B102" s="1">
         <v>10015</v>
       </c>
-      <c r="C102" s="1" t="n">
+      <c r="C102" s="1">
         <v>103</v>
       </c>
       <c r="D102" s="1" t="s">
@@ -1927,14 +2210,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B103" s="1" t="n">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A103" t="s">
+        <v>5</v>
+      </c>
+      <c r="B103" s="1">
         <v>10015</v>
       </c>
-      <c r="C103" s="1" t="n">
+      <c r="C103" s="1">
         <v>104</v>
       </c>
       <c r="D103" s="1" t="s">
@@ -1944,14 +2227,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B104" s="1" t="n">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A104" t="s">
+        <v>5</v>
+      </c>
+      <c r="B104" s="1">
         <v>10015</v>
       </c>
-      <c r="C104" s="1" t="n">
+      <c r="C104" s="1">
         <v>105</v>
       </c>
       <c r="D104" s="1" t="s">
@@ -1961,14 +2244,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B105" s="1" t="n">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A105" t="s">
+        <v>5</v>
+      </c>
+      <c r="B105" s="1">
         <v>10015</v>
       </c>
-      <c r="C105" s="1" t="n">
+      <c r="C105" s="1">
         <v>106</v>
       </c>
       <c r="D105" s="1" t="s">
@@ -1978,14 +2261,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B106" s="1" t="n">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A106" t="s">
+        <v>5</v>
+      </c>
+      <c r="B106" s="1">
         <v>10015</v>
       </c>
-      <c r="C106" s="1" t="n">
+      <c r="C106" s="1">
         <v>107</v>
       </c>
       <c r="D106" s="1" t="s">
@@ -1995,13 +2278,128 @@
         <v>7</v>
       </c>
     </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A107" t="s">
+        <v>15</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C107" s="1">
+        <v>101</v>
+      </c>
+      <c r="D107" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E107" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A108" t="s">
+        <v>15</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C108" s="1">
+        <v>102</v>
+      </c>
+      <c r="D108" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E108" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A109" t="s">
+        <v>15</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C109" s="1">
+        <v>103</v>
+      </c>
+      <c r="D109" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E109" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A110" t="s">
+        <v>15</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C110" s="1">
+        <v>104</v>
+      </c>
+      <c r="D110" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E110" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A111" t="s">
+        <v>15</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C111" s="1">
+        <v>105</v>
+      </c>
+      <c r="D111" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E111" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A112" t="s">
+        <v>15</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C112" s="1">
+        <v>106</v>
+      </c>
+      <c r="D112" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E112" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A113" t="s">
+        <v>15</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C113" s="1">
+        <v>107</v>
+      </c>
+      <c r="D113" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E113" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>